<commit_message>
Done some hotfix to complete project
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schne\Documents\GitHome\MCTG_Brian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDCC624-F998-4792-BB57-EBB2CA98924B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBEF20B-76DA-43BC-89F1-7B1B4BA0ACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="11505" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,6 +773,9 @@
       <c r="A24" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
       <c r="C24" s="6">
         <v>3</v>
       </c>
@@ -792,6 +795,9 @@
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
       <c r="C26" s="6">
         <v>3</v>
       </c>
@@ -807,6 +813,9 @@
       <c r="A29" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
       <c r="C29" s="6">
         <v>4</v>
       </c>
@@ -867,7 +876,9 @@
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B36"/>
+      <c r="B36">
+        <v>3</v>
+      </c>
       <c r="C36" s="6">
         <v>3</v>
       </c>
@@ -916,6 +927,9 @@
       <c r="A42" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
       <c r="C42" s="6">
         <v>5</v>
       </c>
@@ -988,7 +1002,7 @@
       </c>
       <c r="B54" s="2">
         <f>IF(MIN(B9:B16)=1,SUM(B21:B52),0)</f>
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C54" s="2">
         <f>SUM(C21:C52)</f>
@@ -1007,21 +1021,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1153,10 +1152,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1178,19 +1202,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add readme w/ gitlink
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schne\Documents\GitHome\MCTG_Brian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBEF20B-76DA-43BC-89F1-7B1B4BA0ACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877F3667-BAC5-44EC-9B18-895B1555FF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="11505" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -42,12 +42,6 @@
     <t>Review Date:</t>
   </si>
   <si>
-    <t>Student Name:</t>
-  </si>
-  <si>
-    <t>Personal Identifier:</t>
-  </si>
-  <si>
     <t>Must Haves</t>
   </si>
   <si>
@@ -175,6 +169,12 @@
   </si>
   <si>
     <t>Describes design</t>
+  </si>
+  <si>
+    <t>Student Name: Brian Schneider</t>
+  </si>
+  <si>
+    <t>Personal Identifier: if21b072</t>
   </si>
 </sst>
 </file>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,30 +630,30 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -701,7 +701,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -709,7 +709,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -717,28 +717,28 @@
     </row>
     <row r="18" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -760,7 +760,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -793,7 +793,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -804,14 +804,14 @@
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29">
         <v>4</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -833,7 +833,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -855,7 +855,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
       </c>
       <c r="C33" s="6">
         <v>1</v>
@@ -863,7 +866,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -874,7 +877,7 @@
     </row>
     <row r="36" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -885,14 +888,14 @@
     </row>
     <row r="38" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B38"/>
       <c r="C38"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -903,7 +906,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -914,7 +917,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B41">
         <v>5</v>
@@ -925,7 +928,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B42">
         <v>5</v>
@@ -936,21 +939,21 @@
     </row>
     <row r="44" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B44"/>
       <c r="C44" s="6"/>
     </row>
     <row r="46" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C47" s="6">
         <v>1</v>
@@ -958,7 +961,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C48" s="6">
         <v>1</v>
@@ -966,7 +969,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C49" s="6">
         <v>1</v>
@@ -974,7 +977,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C50" s="6">
         <v>1</v>
@@ -982,7 +985,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C51" s="6">
         <v>0.5</v>
@@ -990,7 +993,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="B52">
+        <v>0.5</v>
       </c>
       <c r="C52" s="6">
         <v>0.5</v>
@@ -998,11 +1004,11 @@
     </row>
     <row r="54" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B54" s="2">
         <f>IF(MIN(B9:B16)=1,SUM(B21:B52),0)</f>
-        <v>54</v>
+        <v>55.5</v>
       </c>
       <c r="C54" s="2">
         <f>SUM(C21:C52)</f>
@@ -1021,6 +1027,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1152,35 +1173,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1202,9 +1198,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>